<commit_message>
fix bug after discuss2
</commit_message>
<xml_diff>
--- a/manager/public/assets/tml/client_quotient.xlsx
+++ b/manager/public/assets/tml/client_quotient.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>序号</t>
   </si>
@@ -38,9 +38,6 @@
     <t>投资人姓名</t>
   </si>
   <si>
-    <t>交易金额（万元）</t>
-  </si>
-  <si>
     <t>投资人类型</t>
   </si>
   <si>
@@ -138,6 +135,18 @@
   </si>
   <si>
     <t>中国建设银行上海市宜川支行3</t>
+  </si>
+  <si>
+    <t>xxxxx1</t>
+  </si>
+  <si>
+    <t>yyyyy2</t>
+  </si>
+  <si>
+    <t>zzzzz3</t>
+  </si>
+  <si>
+    <t>交易金额（元）</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -572,37 +581,37 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -610,36 +619,36 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -647,36 +656,36 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -684,40 +693,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>